<commit_message>
Add Breakdown of FOS
</commit_message>
<xml_diff>
--- a/topology_projects_that_comply/applying_changes/ProjectMapping.xlsx
+++ b/topology_projects_that_comply/applying_changes/ProjectMapping.xlsx
@@ -586,7 +586,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ksu</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1562,7 +1562,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.cmu</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2534,7 +2534,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.latech</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2676,7 +2676,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.tufts</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3148,7 +3148,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ku</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -3196,7 +3196,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.duke</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -3336,7 +3336,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.stonybrook</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4188,7 +4188,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.uta</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -4416,7 +4416,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.Jet-EtMiss</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4464,7 +4464,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.louisville</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -5350,7 +5350,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>duke</t>
+          <t>duke.lsst</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -6154,7 +6154,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.B-Physics</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -7002,7 +7002,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.caltech</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -7050,7 +7050,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.purdue</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -8138,7 +8138,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.iastate</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -8322,7 +8322,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.purduecal</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -9820,7 +9820,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.mit</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -10108,7 +10108,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.llnl</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -10668,7 +10668,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ohiostate</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -10760,7 +10760,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.mit</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -11716,7 +11716,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.nyu</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -12748,7 +12748,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.tamu</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.fresnostate</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -13678,7 +13678,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.msu</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -14486,7 +14486,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.Tau</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -14670,7 +14670,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Exotics</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -15554,7 +15554,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.unm</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -15822,7 +15822,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.wayne</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -16338,7 +16338,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.hamptonu</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -16434,7 +16434,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.lbnl</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -17090,7 +17090,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.uoregon</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -17138,7 +17138,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.yale</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -17234,7 +17234,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.utk</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -17378,7 +17378,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Top</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -17614,7 +17614,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ua</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -17802,7 +17802,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.ou</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -18278,7 +18278,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.uchicago</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -18742,7 +18742,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.washington</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -19022,7 +19022,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ucla</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -19354,7 +19354,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>spt</t>
+          <t>spt.all</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -19498,7 +19498,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.neu</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -19546,7 +19546,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.umass</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -20020,7 +20020,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.illinois</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -21054,7 +21054,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.uiowa</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -21290,7 +21290,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.albany</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -22370,7 +22370,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.unl</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -22466,7 +22466,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.cornell</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -22794,7 +22794,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.combined-muon</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -22842,7 +22842,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.slac</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -23350,7 +23350,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.upr</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -24104,7 +24104,7 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.osu</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
@@ -24288,7 +24288,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.smu</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
@@ -24988,7 +24988,7 @@
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.uci</t>
         </is>
       </c>
       <c r="B524" t="inlineStr">
@@ -25036,7 +25036,7 @@
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.fairfield</t>
         </is>
       </c>
       <c r="B525" t="inlineStr">
@@ -25176,7 +25176,7 @@
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.anl</t>
         </is>
       </c>
       <c r="B528" t="inlineStr">
@@ -25876,7 +25876,7 @@
     <row r="543">
       <c r="A543" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.utexas</t>
         </is>
       </c>
       <c r="B543" t="inlineStr">
@@ -26204,7 +26204,7 @@
     <row r="550">
       <c r="A550" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.princeton</t>
         </is>
       </c>
       <c r="B550" t="inlineStr">
@@ -26716,7 +26716,7 @@
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.okstate</t>
         </is>
       </c>
       <c r="B561" t="inlineStr">
@@ -27412,7 +27412,7 @@
     <row r="576">
       <c r="A576" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.upenn</t>
         </is>
       </c>
       <c r="B576" t="inlineStr">
@@ -28526,7 +28526,7 @@
     <row r="600">
       <c r="A600" t="inlineStr">
         <is>
-          <t>osg</t>
+          <t>osg.Ceser</t>
         </is>
       </c>
       <c r="B600" t="n">
@@ -28980,7 +28980,7 @@
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.wisc</t>
         </is>
       </c>
       <c r="B610" t="inlineStr">
@@ -29410,7 +29410,7 @@
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.brown</t>
         </is>
       </c>
       <c r="B619" t="inlineStr">
@@ -29740,7 +29740,7 @@
     <row r="626">
       <c r="A626" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ucsb</t>
         </is>
       </c>
       <c r="B626" t="inlineStr">
@@ -30352,7 +30352,7 @@
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.jhu</t>
         </is>
       </c>
       <c r="B639" t="inlineStr">
@@ -30732,7 +30732,7 @@
     <row r="647">
       <c r="A647" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.bu</t>
         </is>
       </c>
       <c r="B647" t="inlineStr">
@@ -30968,7 +30968,7 @@
     <row r="652">
       <c r="A652" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Monte-Carlo</t>
         </is>
       </c>
       <c r="B652" t="inlineStr">
@@ -31400,7 +31400,7 @@
     <row r="661">
       <c r="A661" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.utdallas</t>
         </is>
       </c>
       <c r="B661" t="inlineStr">
@@ -31584,7 +31584,7 @@
     <row r="665">
       <c r="A665" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.fsu</t>
         </is>
       </c>
       <c r="B665" t="inlineStr">
@@ -33220,7 +33220,7 @@
     <row r="700">
       <c r="A700" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Standard-Model</t>
         </is>
       </c>
       <c r="B700" t="inlineStr">
@@ -33268,7 +33268,7 @@
     <row r="701">
       <c r="A701" t="inlineStr">
         <is>
-          <t>duke</t>
+          <t>duke.ppsa</t>
         </is>
       </c>
       <c r="B701" t="inlineStr">
@@ -34072,7 +34072,7 @@
     <row r="718">
       <c r="A718" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ufl</t>
         </is>
       </c>
       <c r="B718" t="inlineStr">
@@ -34308,7 +34308,7 @@
     <row r="723">
       <c r="A723" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.olemiss</t>
         </is>
       </c>
       <c r="B723" t="inlineStr">
@@ -34448,7 +34448,7 @@
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.umd</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
@@ -36232,7 +36232,7 @@
     <row r="764">
       <c r="A764" t="inlineStr">
         <is>
-          <t>JLAB</t>
+          <t>JLAB.EIC</t>
         </is>
       </c>
       <c r="B764" t="inlineStr">
@@ -36280,7 +36280,7 @@
     <row r="765">
       <c r="A765" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.rice</t>
         </is>
       </c>
       <c r="B765" t="inlineStr">
@@ -36424,7 +36424,7 @@
     <row r="768">
       <c r="A768" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.colorado</t>
         </is>
       </c>
       <c r="B768" t="inlineStr">
@@ -36612,7 +36612,7 @@
     <row r="772">
       <c r="A772" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ucr</t>
         </is>
       </c>
       <c r="B772" t="inlineStr">
@@ -36660,7 +36660,7 @@
     <row r="773">
       <c r="A773" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.E-Gamma</t>
         </is>
       </c>
       <c r="B773" t="inlineStr">
@@ -37040,7 +37040,7 @@
     <row r="781">
       <c r="A781" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.arizona</t>
         </is>
       </c>
       <c r="B781" t="inlineStr">
@@ -37280,7 +37280,7 @@
     <row r="786">
       <c r="A786" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.niu</t>
         </is>
       </c>
       <c r="B786" t="inlineStr">
@@ -37984,7 +37984,7 @@
     <row r="801">
       <c r="A801" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ttu</t>
         </is>
       </c>
       <c r="B801" t="inlineStr">
@@ -38032,7 +38032,7 @@
     <row r="802">
       <c r="A802" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.rochester</t>
         </is>
       </c>
       <c r="B802" t="inlineStr">
@@ -38594,7 +38594,7 @@
     <row r="814">
       <c r="A814" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.northwestern</t>
         </is>
       </c>
       <c r="B814" t="inlineStr">
@@ -38690,7 +38690,7 @@
     <row r="816">
       <c r="A816" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.columbia</t>
         </is>
       </c>
       <c r="B816" t="inlineStr">
@@ -39070,7 +39070,7 @@
     <row r="824">
       <c r="A824" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.uiowa</t>
         </is>
       </c>
       <c r="B824" t="inlineStr">
@@ -39162,7 +39162,7 @@
     <row r="826">
       <c r="A826" t="inlineStr">
         <is>
-          <t>AMNH</t>
+          <t>AMNH.astro</t>
         </is>
       </c>
       <c r="B826" t="inlineStr">
@@ -39478,7 +39478,7 @@
     <row r="833">
       <c r="A833" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ucsd</t>
         </is>
       </c>
       <c r="B833" t="inlineStr">
@@ -39858,7 +39858,7 @@
     <row r="841">
       <c r="A841" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.rockefeller</t>
         </is>
       </c>
       <c r="B841" t="inlineStr">
@@ -40186,7 +40186,7 @@
     <row r="848">
       <c r="A848" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.fiu</t>
         </is>
       </c>
       <c r="B848" t="inlineStr">
@@ -40750,7 +40750,7 @@
     <row r="860">
       <c r="A860" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Inner-Tracking</t>
         </is>
       </c>
       <c r="B860" t="inlineStr">
@@ -40890,7 +40890,7 @@
     <row r="863">
       <c r="A863" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.buffalo</t>
         </is>
       </c>
       <c r="B863" t="inlineStr">
@@ -41506,7 +41506,7 @@
     <row r="876">
       <c r="A876" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.indiana</t>
         </is>
       </c>
       <c r="B876" t="inlineStr">
@@ -42074,7 +42074,7 @@
     <row r="888">
       <c r="A888" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.virginia</t>
         </is>
       </c>
       <c r="B888" t="inlineStr">
@@ -42262,7 +42262,7 @@
     <row r="892">
       <c r="A892" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Flavour-Tagging</t>
         </is>
       </c>
       <c r="B892" t="inlineStr">
@@ -42494,7 +42494,7 @@
     <row r="897">
       <c r="A897" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.bnl</t>
         </is>
       </c>
       <c r="B897" t="inlineStr">
@@ -42678,7 +42678,7 @@
     <row r="901">
       <c r="A901" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.SUSY</t>
         </is>
       </c>
       <c r="B901" t="inlineStr">
@@ -43014,7 +43014,7 @@
     <row r="908">
       <c r="A908" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Heavy-Ions</t>
         </is>
       </c>
       <c r="B908" t="inlineStr">
@@ -43302,7 +43302,7 @@
     <row r="914">
       <c r="A914" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.brandeis</t>
         </is>
       </c>
       <c r="B914" t="inlineStr">
@@ -43994,7 +43994,7 @@
     <row r="929">
       <c r="A929" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.sc</t>
         </is>
       </c>
       <c r="B929" t="inlineStr">
@@ -44418,7 +44418,7 @@
     <row r="938">
       <c r="A938" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.baylor</t>
         </is>
       </c>
       <c r="B938" t="inlineStr">
@@ -44466,7 +44466,7 @@
     <row r="939">
       <c r="A939" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.cern</t>
         </is>
       </c>
       <c r="B939" t="inlineStr">
@@ -44754,7 +44754,7 @@
     <row r="945">
       <c r="A945" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.ucdavis</t>
         </is>
       </c>
       <c r="B945" t="inlineStr">
@@ -45182,7 +45182,7 @@
     <row r="954">
       <c r="A954" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.USAtlas-TechSupport</t>
         </is>
       </c>
       <c r="B954" t="inlineStr">
@@ -45414,7 +45414,7 @@
     <row r="959">
       <c r="A959" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.wisc</t>
         </is>
       </c>
       <c r="B959" t="inlineStr">
@@ -45646,7 +45646,7 @@
     <row r="964">
       <c r="A964" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.vanderbilt</t>
         </is>
       </c>
       <c r="B964" t="inlineStr">
@@ -46642,7 +46642,7 @@
     <row r="985">
       <c r="A985" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.ucsc</t>
         </is>
       </c>
       <c r="B985" t="inlineStr">
@@ -46930,7 +46930,7 @@
     <row r="991">
       <c r="A991" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.umn</t>
         </is>
       </c>
       <c r="B991" t="inlineStr">
@@ -48054,7 +48054,7 @@
     <row r="1015">
       <c r="A1015" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.fnal</t>
         </is>
       </c>
       <c r="B1015" t="inlineStr">
@@ -48338,7 +48338,7 @@
     <row r="1021">
       <c r="A1021" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.pitt</t>
         </is>
       </c>
       <c r="B1021" t="inlineStr">
@@ -48998,7 +48998,7 @@
     <row r="1035">
       <c r="A1035" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.nd</t>
         </is>
       </c>
       <c r="B1035" t="inlineStr">
@@ -49658,7 +49658,7 @@
     <row r="1049">
       <c r="A1049" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.fit</t>
         </is>
       </c>
       <c r="B1049" t="inlineStr">
@@ -50126,7 +50126,7 @@
     <row r="1059">
       <c r="A1059" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.wg.Higgs</t>
         </is>
       </c>
       <c r="B1059" t="inlineStr">
@@ -50502,7 +50502,7 @@
     <row r="1067">
       <c r="A1067" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.rutgers</t>
         </is>
       </c>
       <c r="B1067" t="inlineStr">
@@ -50646,7 +50646,7 @@
     <row r="1070">
       <c r="A1070" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.harvard</t>
         </is>
       </c>
       <c r="B1070" t="inlineStr">
@@ -50930,7 +50930,7 @@
     <row r="1076">
       <c r="A1076" t="inlineStr">
         <is>
-          <t>atlas</t>
+          <t>atlas.org.bu</t>
         </is>
       </c>
       <c r="B1076" t="inlineStr">
@@ -51582,7 +51582,7 @@
     <row r="1090">
       <c r="A1090" t="inlineStr">
         <is>
-          <t>cms</t>
+          <t>cms.org.uic</t>
         </is>
       </c>
       <c r="B1090" t="inlineStr">

</xml_diff>